<commit_message>
TC_MISC_GA_WH_Yes_01 case flow completed
</commit_message>
<xml_diff>
--- a/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/Payer_Data_Import_Template.xlsx
+++ b/Demo_working/Tax1099Automation-master/Demo_working/src/test/resources/TestData/Payer_Data_Import_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Payer Type</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Sridevi47@zenwork.com</t>
+  </si>
+  <si>
+    <t>181703635</t>
+  </si>
+  <si>
+    <t>Imported93496618</t>
+  </si>
+  <si>
+    <t>Sridevi73@zenwork.com</t>
   </si>
 </sst>
 </file>
@@ -651,10 +660,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>24</v>
@@ -678,7 +687,7 @@
         <v>1234567822</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S2" s="6">
         <v>222</v>

</xml_diff>